<commit_message>
Updated Links & Pdf's
Outer PDF's are added
And CD Data-Flow-Analysis links were modifies
</commit_message>
<xml_diff>
--- a/Prepared_Links/Subjects_Concepts_Links.xlsx
+++ b/Prepared_Links/Subjects_Concepts_Links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GATE\GATE_CS_2021\Prepared_Links\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8554251-833A-4281-B740-1A4478910A7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D2FBAC-603E-41BF-937B-987A13F0FBC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3252" yWindow="684" windowWidth="18060" windowHeight="11460" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DLD" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="93">
   <si>
     <t>Chapter</t>
   </si>
@@ -270,6 +270,51 @@
   </si>
   <si>
     <t>without Local Procedures</t>
+  </si>
+  <si>
+    <t>Intermediate Code</t>
+  </si>
+  <si>
+    <t>Three Address code</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=yFVCw0N0nxo&amp;ab_channel=SudhakarAtchala</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sv5Qmq8Hjz4&amp;t=140s&amp;ab_channel=SudhakarAtchala</t>
+  </si>
+  <si>
+    <t>Quadrples, Triples,Indirect Triples</t>
+  </si>
+  <si>
+    <t>Code Optimization</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=yHZFVz6TVmI&amp;list=PLXj4XH7LcRfC9pGMWuM6UWE3V4YZ9TZzM&amp;index=51&amp;ab_channel=SudhakarAtchala</t>
+  </si>
+  <si>
+    <t>Constant Propagation</t>
+  </si>
+  <si>
+    <t>Common Subexpression Elimination</t>
+  </si>
+  <si>
+    <t>https://www.gatevidyalay.com/code-optimization-techniques/</t>
+  </si>
+  <si>
+    <t>Reading Material</t>
+  </si>
+  <si>
+    <t>Data-Flow-Analysis</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=OROXJ9-wUQE&amp;t=1600s&amp;ab_channel=MayurNaik</t>
+  </si>
+  <si>
+    <t>Tutorials Point</t>
+  </si>
+  <si>
+    <t>https://youtu.be/0hU5-aLtaxo</t>
   </si>
 </sst>
 </file>
@@ -1046,16 +1091,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD7F91D-C200-4A05-BE96-72024D666C01}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="134" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1100,6 +1145,17 @@
         <v>67</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
@@ -1135,7 +1191,62 @@
         <v>70</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C15:C16"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{602D0923-A61C-402B-8BD5-EFE540C13BDA}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Noisy vs Noiseless Channel capacity links updated
</commit_message>
<xml_diff>
--- a/Prepared_Links/Subjects_Concepts_Links.xlsx
+++ b/Prepared_Links/Subjects_Concepts_Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GATE\GATE_CS_2021\Prepared_Links\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DD731D-8F14-4AE4-8CD2-12B2DDC10134}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F24FFFA-81A2-4C3A-941D-F07DB71590B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="128">
   <si>
     <t>Chapter</t>
   </si>
@@ -409,6 +409,21 @@
   </si>
   <si>
     <t>https://www.youtube.com/playlist?list=PLEbnTDJUr_If_GCGDEOYensUC5Ur-L9MR</t>
+  </si>
+  <si>
+    <t>Noisy vs Noiseless</t>
+  </si>
+  <si>
+    <t>Maximum Data rate</t>
+  </si>
+  <si>
+    <t>Bit rate vs Baud rate</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/difference-btween-bit-rate-and-baud-rate/?ref=lbp</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/maximum-data-rate-channel-capacity-for-noiseless-and-noisy-channels/?ref=lbp</t>
   </si>
 </sst>
 </file>
@@ -1374,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35654C6F-8054-43D7-A782-339CF9F13D12}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1521,6 +1536,25 @@
       </c>
       <c r="C18" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DBMS & CN Links updated
</commit_message>
<xml_diff>
--- a/Prepared_Links/Subjects_Concepts_Links.xlsx
+++ b/Prepared_Links/Subjects_Concepts_Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GATE\GATE_CS_2021\Prepared_Links\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F24FFFA-81A2-4C3A-941D-F07DB71590B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42014E4-6F4B-4700-BF33-7E7B54F75AB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,8 @@
     <sheet name="TOC" sheetId="4" r:id="rId4"/>
     <sheet name="CD" sheetId="5" r:id="rId5"/>
     <sheet name="CN" sheetId="6" r:id="rId6"/>
+    <sheet name="OS" sheetId="7" r:id="rId7"/>
+    <sheet name="DBMS" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="136">
   <si>
     <t>Chapter</t>
   </si>
@@ -424,6 +426,30 @@
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/maximum-data-rate-channel-capacity-for-noiseless-and-noisy-channels/?ref=lbp</t>
+  </si>
+  <si>
+    <t>Process Management</t>
+  </si>
+  <si>
+    <t>Schedling Algorithms</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLEbnTDJUr_If_BnzJkkN_J0Tl3iXTL8vq</t>
+  </si>
+  <si>
+    <t>Article from JavaTpoint</t>
+  </si>
+  <si>
+    <t>https://www.javatpoint.com/os-tutorial</t>
+  </si>
+  <si>
+    <t>LAN</t>
+  </si>
+  <si>
+    <t>http://www.cs.montana.edu/~halla/csci466/lectures/lec10-2.7-token.html</t>
+  </si>
+  <si>
+    <t>Token Ring (**Priority Scheme)</t>
   </si>
 </sst>
 </file>
@@ -1389,16 +1415,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35654C6F-8054-43D7-A782-339CF9F13D12}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="114.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1555,6 +1581,17 @@
       </c>
       <c r="C23" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1573,4 +1610,83 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D0BDCB1-D058-47BA-8C94-2B2AC8796618}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180D80CD-E20F-4904-A414-A2AD6878D6F6}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>